<commit_message>
Local Excel: key error: cutoff
</commit_message>
<xml_diff>
--- a/final_cutoff.xlsx
+++ b/final_cutoff.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\campussathi\pref-list\pref-list-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE825B4-5CE8-4FFB-AC6C-BCD259410AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A844931-3A83-43B1-AC16-6B8EB10AD33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1393,13 +1393,13 @@
     <t>Janata Shikshan Prasarak Mandal</t>
   </si>
   <si>
-    <t>Cutoff open</t>
-  </si>
-  <si>
     <t>Technical Textiles</t>
   </si>
   <si>
     <t>Architectural Assistantship</t>
+  </si>
+  <si>
+    <t>Cutoff</t>
   </si>
 </sst>
 </file>
@@ -1671,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:G1828"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1153" workbookViewId="0">
-      <selection activeCell="G1175" sqref="G1175"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1704,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -10565,7 +10565,7 @@
         <v>89510</v>
       </c>
       <c r="F387" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G387" s="1">
         <v>68.473714000000001</v>
@@ -12451,7 +12451,7 @@
         <v>46310</v>
       </c>
       <c r="F469" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G469" s="1">
         <v>23.576740999999998</v>

</xml_diff>